<commit_message>
added get user info API
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062CDB99-B707-484D-853C-5A4B3F3FF0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D185BD4F-316D-480E-A530-838B71E9D243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
   <si>
     <t>URI</t>
   </si>
@@ -352,7 +352,10 @@
     <t>User Obj</t>
   </si>
   <si>
-    <t>login ussing email / username, and password</t>
+    <t>login using email / username, and password</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,6 +741,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -755,6 +761,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -792,6 +801,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -812,6 +824,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -829,6 +844,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -839,7 +857,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
added find export on events
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECFA185-CD97-45B3-9A52-2C2A613FE820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC381B36-5F2C-4CF3-BCE7-B7FA849358D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
   <si>
     <t>URI</t>
   </si>
@@ -85,9 +85,6 @@
     <t>patch</t>
   </si>
   <si>
-    <t>get user stats</t>
-  </si>
-  <si>
     <t>/users/:userID/stats</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Stats Obj</t>
   </si>
   <si>
-    <t>get user stats for the season</t>
-  </si>
-  <si>
     <t>update user stats for the season</t>
   </si>
   <si>
@@ -115,27 +109,12 @@
     <t>&lt;filtered USERS collection&gt;</t>
   </si>
   <si>
-    <t>/users/:userID/stats?season=&lt;int&gt;</t>
-  </si>
-  <si>
     <t>/events/?userID=&lt;id&gt;</t>
   </si>
   <si>
-    <t>/events/?type=&lt;type&gt;</t>
-  </si>
-  <si>
-    <t>get events based on type</t>
-  </si>
-  <si>
     <t>get all joined events of the user</t>
   </si>
   <si>
-    <t>get events based on status</t>
-  </si>
-  <si>
-    <t>/events/?status=&lt;status&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">get </t>
   </si>
   <si>
@@ -334,12 +313,6 @@
     <t>admin / hosted 10 events</t>
   </si>
   <si>
-    <t>/events/?hostedBy=&lt;id&gt;</t>
-  </si>
-  <si>
-    <t>/events/?joinedBy=&lt;id&gt;</t>
-  </si>
-  <si>
     <t>get all the events related to the user</t>
   </si>
   <si>
@@ -362,6 +335,33 @@
   </si>
   <si>
     <t>on success</t>
+  </si>
+  <si>
+    <t>get all user stats</t>
+  </si>
+  <si>
+    <t>/users/:userID/stats/:season/:type</t>
+  </si>
+  <si>
+    <t>/users/:userID/stats?season=&lt;int&gt;&amp;type=&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>not sure if this is needed</t>
+  </si>
+  <si>
+    <t>get user stats for the season/type</t>
+  </si>
+  <si>
+    <t>/events/hostedBy/:userId</t>
+  </si>
+  <si>
+    <t>/events/joinedBy/:userId</t>
+  </si>
+  <si>
+    <t>/events/?type=&lt;string&gt;&amp;status=&lt;string&gt;&amp;libero=&lt;boolean&gt;&amp;season=&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>get events based on type / status / libero / season</t>
   </si>
 </sst>
 </file>
@@ -385,12 +385,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -405,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +420,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -733,12 +743,13 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="34.109375" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
@@ -748,8 +759,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>106</v>
+      <c r="A1" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -764,15 +775,15 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>102</v>
+      <c r="A2" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -790,12 +801,12 @@
         <v>200</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>102</v>
+      <c r="A3" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -813,18 +824,18 @@
         <v>201</v>
       </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>102</v>
+      <c r="A4" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -836,21 +847,21 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>102</v>
+      <c r="A5" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -862,38 +873,41 @@
         <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>102</v>
+      <c r="A6" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3">
         <v>200</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -901,16 +915,22 @@
       <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F7" s="3">
+        <v>200</v>
+      </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -918,16 +938,22 @@
       <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F8" s="3">
+        <v>200</v>
+      </c>
       <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -936,18 +962,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>102</v>
+      <c r="A10" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -959,32 +985,37 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
-        <v>62</v>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -993,15 +1024,15 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1010,167 +1041,150 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="F18" s="3">
         <v>200</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>102</v>
+      <c r="A19" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3">
         <v>201</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>102</v>
+      <c r="A20" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F20" s="3">
         <v>204</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>102</v>
+      <c r="A21" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F21" s="3">
         <v>204</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>102</v>
+      <c r="A22" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>102</v>
+      <c r="A23" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1182,35 +1196,35 @@
         <v>204</v>
       </c>
       <c r="G23" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1219,15 +1233,15 @@
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1236,15 +1250,15 @@
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1253,83 +1267,83 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G31" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -1338,15 +1352,15 @@
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1355,15 +1369,15 @@
         <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1372,15 +1386,15 @@
         <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1389,15 +1403,15 @@
         <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1406,15 +1420,15 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -1423,15 +1437,15 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -1440,15 +1454,15 @@
         <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -1457,15 +1471,15 @@
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1474,15 +1488,15 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -1491,15 +1505,15 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -1508,75 +1522,75 @@
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G48" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G49" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D50" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G50" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G51" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converted position to positionpreference
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC381B36-5F2C-4CF3-BCE7-B7FA849358D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A3FF0-D644-4CA5-9949-38D97DC6A8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="112">
   <si>
     <t>URI</t>
   </si>
@@ -157,12 +157,6 @@
     <t>/events/:eventID/reservations</t>
   </si>
   <si>
-    <t>see all event reservation groups</t>
-  </si>
-  <si>
-    <t>see event reservation group</t>
-  </si>
-  <si>
     <t>see event reservation group member</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>get all hosted events of the user</t>
   </si>
   <si>
-    <t>/events/:eventID/reservations/:groupID</t>
-  </si>
-  <si>
     <t>/events/:eventID/reservations/:groupID/:reservationID</t>
   </si>
   <si>
@@ -358,10 +349,28 @@
     <t>/events/joinedBy/:userId</t>
   </si>
   <si>
-    <t>/events/?type=&lt;string&gt;&amp;status=&lt;string&gt;&amp;libero=&lt;boolean&gt;&amp;season=&lt;int&gt;</t>
-  </si>
-  <si>
     <t>get events based on type / status / libero / season</t>
+  </si>
+  <si>
+    <t>/events/&lt;joined(hosted)By/:userId/&gt;?type=&lt;string&gt;&amp;status=&lt;string&gt;&amp;libero=&lt;boolean&gt;&amp;season=&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>see event reservation group / reservation id</t>
+  </si>
+  <si>
+    <t>get reservations of a user</t>
+  </si>
+  <si>
+    <t>/reservations/by/:userId/?populate=true</t>
+  </si>
+  <si>
+    <t>see all event reservations</t>
+  </si>
+  <si>
+    <t>/events/:eventID/reservations/?groupId=&lt;groupId&gt;&amp;reservationId=&lt;reservationId&gt;</t>
+  </si>
+  <si>
+    <t>/events/:eventID/reservations?grouped=true&amp;groupId=&lt;groupId&gt;&amp;reservationId=&lt;reservationId&gt;</t>
   </si>
 </sst>
 </file>
@@ -740,18 +749,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64DEFC9-EAB2-45D7-9C2E-1AA1A2A50309}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="57" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="57" style="3" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
     <col min="5" max="5" width="21.109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.21875" style="3" customWidth="1"/>
@@ -760,12 +769,12 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -775,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
@@ -783,12 +792,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -806,12 +815,12 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -824,17 +833,17 @@
         <v>201</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
@@ -847,20 +856,20 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
@@ -873,17 +882,17 @@
         <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
@@ -896,17 +905,17 @@
         <v>200</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
@@ -924,13 +933,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
+        <v>90</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -947,13 +956,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>101</v>
+      <c r="C9" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -965,15 +974,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" t="s">
-        <v>94</v>
+      <c r="C10" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -985,15 +994,15 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="B12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1004,18 +1013,18 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1027,29 +1036,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" t="s">
-        <v>107</v>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1063,12 +1077,12 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D18" t="s">
@@ -1086,12 +1100,12 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D19" t="s">
@@ -1109,13 +1123,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
+        <v>90</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1132,12 +1146,12 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D21" t="s">
@@ -1153,17 +1167,17 @@
         <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D22" t="s">
@@ -1178,12 +1192,12 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="s">
@@ -1199,14 +1213,17 @@
         <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="A25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D25" t="s">
@@ -1215,16 +1232,22 @@
       <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="F25" s="3">
+        <v>201</v>
+      </c>
       <c r="G25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1232,118 +1255,125 @@
       <c r="E27" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="F27" s="3">
+        <v>200</v>
+      </c>
       <c r="G27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C31" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
+      <c r="B35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -1352,15 +1382,15 @@
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>60</v>
+      <c r="B36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1369,15 +1399,15 @@
         <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
+      <c r="B37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -1386,15 +1416,15 @@
         <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1403,15 +1433,15 @@
         <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>58</v>
+      <c r="B39" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1420,15 +1450,15 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" t="s">
-        <v>66</v>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -1437,15 +1467,15 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
+      <c r="B41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -1454,15 +1484,15 @@
         <v>7</v>
       </c>
       <c r="G41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
+      <c r="C42" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -1471,15 +1501,15 @@
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" t="s">
-        <v>52</v>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1488,14 +1518,14 @@
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
@@ -1505,14 +1535,14 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D46" t="s">
@@ -1522,75 +1552,83 @@
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G49" t="s">
         <v>83</v>
       </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D48" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="C50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G48" t="s">
+      <c r="C51" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="C52" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C50" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>90</v>
-      </c>
-      <c r="C51" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G51" t="s">
-        <v>86</v>
+      <c r="G52" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added event schedules model
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A3FF0-D644-4CA5-9949-38D97DC6A8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD202C03-B2D3-4C13-8AE6-9E8825A93ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="122">
   <si>
     <t>URI</t>
   </si>
@@ -217,9 +217,6 @@
     <t>see specific event team</t>
   </si>
   <si>
-    <t>Teams Obj</t>
-  </si>
-  <si>
     <t>Team Obj</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>Schedule Obj</t>
   </si>
   <si>
-    <t>modify event teams</t>
-  </si>
-  <si>
     <t>modify specific event team</t>
   </si>
   <si>
@@ -256,18 +250,9 @@
     <t>add event team</t>
   </si>
   <si>
-    <t>add event schedule</t>
-  </si>
-  <si>
     <t>delete event team</t>
   </si>
   <si>
-    <t>Team Obj and Teams Obj</t>
-  </si>
-  <si>
-    <t>Teams Obj and Team Obj</t>
-  </si>
-  <si>
     <t>Schedules Obj and Schedule Obj</t>
   </si>
   <si>
@@ -371,6 +356,51 @@
   </si>
   <si>
     <t>/events/:eventID/reservations?grouped=true&amp;groupId=&lt;groupId&gt;&amp;reservationId=&lt;reservationId&gt;</t>
+  </si>
+  <si>
+    <t>event must be open</t>
+  </si>
+  <si>
+    <t>admin / host user / user that belongs to a team of the event</t>
+  </si>
+  <si>
+    <t>[Team Obj]</t>
+  </si>
+  <si>
+    <t>/events/:eventID/teams?populate=&lt;boolean&gt;</t>
+  </si>
+  <si>
+    <t>not sure if needed</t>
+  </si>
+  <si>
+    <t>/events/:eventID/schedule</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>add/update event schedule</t>
+  </si>
+  <si>
+    <t>/events/:eventID/schedule?populate=&lt;boolean&gt;</t>
+  </si>
+  <si>
+    <t>teams Obj</t>
+  </si>
+  <si>
+    <t>teams Obj and Team Obj</t>
+  </si>
+  <si>
+    <t>Team Obj and teams Obj</t>
+  </si>
+  <si>
+    <t>under put</t>
+  </si>
+  <si>
+    <t>add/update teams</t>
+  </si>
+  <si>
+    <t>/events/:eventID/schedule/:scheduleID</t>
   </si>
 </sst>
 </file>
@@ -752,8 +782,8 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +799,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -784,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
@@ -792,7 +822,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -815,7 +845,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -833,12 +863,12 @@
         <v>201</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -856,7 +886,7 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -864,7 +894,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -882,12 +912,12 @@
         <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -905,15 +935,15 @@
         <v>200</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -933,13 +963,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -956,13 +986,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -976,13 +1006,13 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -994,13 +1024,13 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>24</v>
@@ -1018,13 +1048,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1042,7 +1072,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
@@ -1057,13 +1087,13 @@
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1077,7 +1107,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -1100,7 +1130,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>29</v>
@@ -1123,7 +1153,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
@@ -1146,7 +1176,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>32</v>
@@ -1167,12 +1197,12 @@
         <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>58</v>
@@ -1192,7 +1222,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -1213,12 +1243,12 @@
         <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>36</v>
@@ -1241,13 +1271,13 @@
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1265,10 +1295,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>5</v>
@@ -1301,23 +1331,29 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="B32" s="3" t="s">
         <v>59</v>
       </c>
@@ -1331,15 +1367,18 @@
         <v>56</v>
       </c>
       <c r="G32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1348,15 +1387,18 @@
         <v>56</v>
       </c>
       <c r="G33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="C34" s="3" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
@@ -1365,146 +1407,162 @@
         <v>56</v>
       </c>
       <c r="G34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="3" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C39" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="5"/>
+      <c r="G39" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B40" s="3" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="F41" s="5"/>
+      <c r="G41" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F42" s="5"/>
+      <c r="G42" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>48</v>
       </c>
@@ -1520,8 +1578,11 @@
       <c r="G44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
         <v>46</v>
       </c>
@@ -1538,7 +1599,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>47</v>
       </c>
@@ -1555,80 +1616,80 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G49" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G50" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G52" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added matchrecords object model
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD202C03-B2D3-4C13-8AE6-9E8825A93ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50453C-3636-48F9-936D-E294DEB8C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
   <si>
     <t>URI</t>
   </si>
@@ -154,9 +154,6 @@
     <t>/reservations/:reservationID</t>
   </si>
   <si>
-    <t>/events/:eventID/reservations</t>
-  </si>
-  <si>
     <t>see event reservation group member</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>cancel reservation</t>
   </si>
   <si>
-    <t>/reservations/:reservationID/cancel</t>
-  </si>
-  <si>
     <t>cancel event</t>
   </si>
   <si>
@@ -401,6 +395,66 @@
   </si>
   <si>
     <t>/events/:eventID/schedule/:scheduleID</t>
+  </si>
+  <si>
+    <t>/events/:eventID/reservations/</t>
+  </si>
+  <si>
+    <t>/events/:eventId/reservations/cancel</t>
+  </si>
+  <si>
+    <t>anyone who signed up</t>
+  </si>
+  <si>
+    <t>add match record</t>
+  </si>
+  <si>
+    <t>admin / host</t>
+  </si>
+  <si>
+    <t>Match Record Obj</t>
+  </si>
+  <si>
+    <t>modify match record</t>
+  </si>
+  <si>
+    <t>delete match record</t>
+  </si>
+  <si>
+    <t>/events/:eventId/matchrecords/</t>
+  </si>
+  <si>
+    <t>/events/:eventId/matchrecords/:matchrecordId</t>
+  </si>
+  <si>
+    <t>get event matchrecords</t>
+  </si>
+  <si>
+    <t>/events/:eventId/matchrecords</t>
+  </si>
+  <si>
+    <t>get user matchrecords</t>
+  </si>
+  <si>
+    <t>/users/:userId/matchrecords</t>
+  </si>
+  <si>
+    <t>all logged user</t>
+  </si>
+  <si>
+    <t>admin / same user</t>
+  </si>
+  <si>
+    <t>[Match Record Obj]</t>
+  </si>
+  <si>
+    <t>coded</t>
+  </si>
+  <si>
+    <t>/events/:eventId/matchrecords/of/:userId</t>
+  </si>
+  <si>
+    <t>get event matchrecords of specific user</t>
   </si>
 </sst>
 </file>
@@ -779,11 +833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64DEFC9-EAB2-45D7-9C2E-1AA1A2A50309}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,12 +848,12 @@
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
     <col min="5" max="5" width="21.109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.21875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -814,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
@@ -822,7 +876,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -845,7 +899,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -863,12 +917,12 @@
         <v>201</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -886,15 +940,15 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -912,12 +966,12 @@
         <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -935,15 +989,15 @@
         <v>200</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -963,13 +1017,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -986,13 +1040,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1006,13 +1060,13 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1024,13 +1078,13 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>24</v>
@@ -1043,18 +1097,18 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1072,7 +1126,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
@@ -1082,18 +1136,18 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1107,7 +1161,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -1130,7 +1184,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>29</v>
@@ -1153,13 +1207,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1176,7 +1230,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>32</v>
@@ -1197,15 +1251,15 @@
         <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>33</v>
@@ -1222,7 +1276,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -1243,18 +1297,18 @@
         <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1266,18 +1320,18 @@
         <v>201</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1289,16 +1343,16 @@
         <v>200</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>5</v>
@@ -1308,16 +1362,16 @@
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>5</v>
@@ -1327,113 +1381,116 @@
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" t="s">
         <v>61</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G33" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>15</v>
@@ -1443,36 +1500,36 @@
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>15</v>
@@ -1482,16 +1539,16 @@
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -1501,36 +1558,36 @@
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>12</v>
@@ -1540,16 +1597,16 @@
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>12</v>
@@ -1559,32 +1616,38 @@
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B44" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="G44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B45" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>38</v>
@@ -1596,12 +1659,15 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B46" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>38</v>
@@ -1613,83 +1679,209 @@
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B47" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="G49" t="s">
         <v>76</v>
       </c>
-      <c r="D49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G49" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B50" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="C50" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="C51" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G52" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added certificates and added positionpreferencemodel
</commit_message>
<xml_diff>
--- a/API list.xlsx
+++ b/API list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vintatech\Desktop\VPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50453C-3636-48F9-936D-E294DEB8C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AA0BD-30F0-4C4D-9051-BBB245E58365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DDB1F74E-B6D2-4F5B-85DB-F848F04CBEE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="REST API" sheetId="1" r:id="rId1"/>
+    <sheet name="TODO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="144">
   <si>
     <t>URI</t>
   </si>
@@ -280,9 +281,6 @@
     <t>delete venue</t>
   </si>
   <si>
-    <t>admin / hosted 10 events</t>
-  </si>
-  <si>
     <t>get all the events related to the user</t>
   </si>
   <si>
@@ -439,9 +437,6 @@
     <t>/users/:userId/matchrecords</t>
   </si>
   <si>
-    <t>all logged user</t>
-  </si>
-  <si>
     <t>admin / same user</t>
   </si>
   <si>
@@ -455,6 +450,24 @@
   </si>
   <si>
     <t>get event matchrecords of specific user</t>
+  </si>
+  <si>
+    <t>get venue details</t>
+  </si>
+  <si>
+    <t>admin / author</t>
+  </si>
+  <si>
+    <t>/venues?author=&lt;ObjectId&gt;</t>
+  </si>
+  <si>
+    <t>FrontEnd</t>
+  </si>
+  <si>
+    <t>Save jwt tokens after succesful login</t>
+  </si>
+  <si>
+    <t>Test APIs and mapping to objects</t>
   </si>
 </sst>
 </file>
@@ -833,11 +846,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64DEFC9-EAB2-45D7-9C2E-1AA1A2A50309}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +866,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -868,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
@@ -876,7 +889,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -899,7 +912,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -917,12 +930,12 @@
         <v>201</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -940,7 +953,7 @@
         <v>204</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
@@ -948,7 +961,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -966,12 +979,12 @@
         <v>204</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -989,15 +1002,15 @@
         <v>200</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -1017,13 +1030,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1040,13 +1053,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1060,13 +1073,13 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1078,13 +1091,13 @@
         <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>24</v>
@@ -1102,13 +1115,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1126,7 +1139,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
@@ -1141,13 +1154,13 @@
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1161,7 +1174,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -1184,7 +1197,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>29</v>
@@ -1207,7 +1220,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>48</v>
@@ -1230,7 +1243,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>32</v>
@@ -1251,12 +1264,12 @@
         <v>31</v>
       </c>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>56</v>
@@ -1276,7 +1289,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -1302,13 +1315,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1325,13 +1338,13 @@
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1349,10 +1362,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>5</v>
@@ -1386,27 +1399,27 @@
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" t="s">
         <v>106</v>
-      </c>
-      <c r="G31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>57</v>
@@ -1426,13 +1439,13 @@
     </row>
     <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1446,13 +1459,13 @@
     </row>
     <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
@@ -1466,22 +1479,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1505,7 +1518,7 @@
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>66</v>
@@ -1523,7 +1536,7 @@
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>67</v>
@@ -1558,21 +1571,21 @@
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
         <v>110</v>
-      </c>
-      <c r="D40" t="s">
-        <v>111</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>7</v>
@@ -1597,7 +1610,7 @@
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1621,30 +1634,30 @@
     </row>
     <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="G44" t="s">
         <v>40</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>45</v>
@@ -1664,7 +1677,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>46</v>
@@ -1684,13 +1697,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -1700,11 +1713,14 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -1716,32 +1732,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="B50" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>9</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51" t="s">
-        <v>15</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>75</v>
@@ -1751,141 +1767,197 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G52" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>125</v>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G53" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D58" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>135</v>
+      <c r="C60" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A19199B-076D-4DCF-946F-E2F9F6FF4239}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>